<commit_message>
Correção da orientação em PVs que não possuem nível
</commit_message>
<xml_diff>
--- a/pvs.xlsx
+++ b/pvs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Iniciação Científica\PV_generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Iniciação Científica\Concrete-Instrum-Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B806558-5FB0-43BE-A844-A105EFC206ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676EEF39-5CF3-4C60-8DE0-85A47DFD0502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8C664926-5403-41C4-B638-B597EA4F600E}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7875" xr2:uid="{8C664926-5403-41C4-B638-B597EA4F600E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3235" uniqueCount="1413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3223" uniqueCount="1413">
   <si>
     <t>A</t>
   </si>
@@ -4279,7 +4279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4306,6 +4306,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4327,7 +4335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4345,6 +4353,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4674,8 +4685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270F984E-E2EF-4600-9BDF-C6DAF7FA9D6F}">
   <dimension ref="A1:I413"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K109" sqref="K109"/>
+    <sheetView tabSelected="1" topLeftCell="A379" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G381" sqref="G381:G388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13057,9 +13068,7 @@
       <c r="F322" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G322" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G322" s="4"/>
       <c r="H322" s="5">
         <v>26</v>
       </c>
@@ -13083,9 +13092,7 @@
       <c r="F323" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G323" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G323" s="4"/>
       <c r="H323" s="5">
         <v>26</v>
       </c>
@@ -13109,9 +13116,7 @@
       <c r="F324" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G324" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G324" s="4"/>
       <c r="H324" s="5">
         <v>26</v>
       </c>
@@ -13135,9 +13140,7 @@
       <c r="F325" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G325" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G325" s="4"/>
       <c r="H325" s="5">
         <v>26</v>
       </c>
@@ -14591,9 +14594,7 @@
       <c r="F381" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G381" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G381" s="7"/>
       <c r="H381" s="5">
         <v>25</v>
       </c>
@@ -14617,9 +14618,7 @@
       <c r="F382" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G382" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G382" s="7"/>
       <c r="H382" s="5">
         <v>25</v>
       </c>
@@ -14643,9 +14642,7 @@
       <c r="F383" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G383" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G383" s="7"/>
       <c r="H383" s="5">
         <v>25</v>
       </c>
@@ -14669,9 +14666,7 @@
       <c r="F384" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G384" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G384" s="7"/>
       <c r="H384" s="5">
         <v>25</v>
       </c>
@@ -14695,9 +14690,7 @@
       <c r="F385" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G385" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G385" s="7"/>
       <c r="H385" s="5">
         <v>25</v>
       </c>
@@ -14721,9 +14714,7 @@
       <c r="F386" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G386" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G386" s="7"/>
       <c r="H386" s="5">
         <v>25</v>
       </c>
@@ -14747,9 +14738,7 @@
       <c r="F387" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G387" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G387" s="7"/>
       <c r="H387" s="5">
         <v>25</v>
       </c>
@@ -14773,9 +14762,7 @@
       <c r="F388" s="4" t="s">
         <v>808</v>
       </c>
-      <c r="G388" s="4" t="s">
-        <v>805</v>
-      </c>
+      <c r="G388" s="7"/>
       <c r="H388" s="5">
         <v>25</v>
       </c>

</xml_diff>